<commit_message>
temporary fixes to files
</commit_message>
<xml_diff>
--- a/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
+++ b/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eltco\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\elec\BPHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8F2437-B3C4-4D9A-838D-B780E42A4C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA8D175-3AEF-4C36-AD41-9C0C52054783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6375" yWindow="660" windowWidth="22125" windowHeight="17175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -543,18 +543,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,27 +562,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
   </sheetData>
@@ -599,120 +599,125 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1">
+        <v>2019</v>
+      </c>
+      <c r="C1">
         <v>2020</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2021</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2022</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2023</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2024</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2025</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>2026</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>2027</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>2028</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2029</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>2030</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2031</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>2032</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>2033</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>2034</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>2035</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>2036</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2037</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>2038</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>2039</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <v>2040</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>2041</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>2042</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>2043</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>2044</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>2045</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>2046</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>2047</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <v>2048</v>
       </c>
-      <c r="AE1">
+      <c r="AF1">
         <v>2049</v>
       </c>
-      <c r="AF1">
+      <c r="AG1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4">
+        <f>C2</f>
         <v>174</v>
       </c>
       <c r="C2" s="4">
@@ -805,7 +810,10 @@
       <c r="AF2" s="4">
         <v>174</v>
       </c>
-      <c r="AG2" s="4"/>
+      <c r="AG2" s="4">
+        <v>174</v>
+      </c>
+      <c r="AH2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -813,23 +821,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </of2ed5e60f3c4f8984f283882cb94320>
-    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ff7c4ad8664a4671b57370e258acad6a>
-    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l787e5950a9249679d0130235a9a791b>
-    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1093,22 +1090,60 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </of2ed5e60f3c4f8984f283882cb94320>
+    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ff7c4ad8664a4671b57370e258acad6a>
+    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l787e5950a9249679d0130235a9a791b>
+    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCB44BB-DC09-4176-A64A-B3802CEA3A76}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B9A3521-3DB4-4F71-B9FE-11018E672020}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10D9DACC-227F-4DB0-98AB-5EBF381C491B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10D9DACC-227F-4DB0-98AB-5EBF381C491B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
+    <ds:schemaRef ds:uri="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B9A3521-3DB4-4F71-B9FE-11018E672020}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCB44BB-DC09-4176-A64A-B3802CEA3A76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>